<commit_message>
05.05.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Others/Price list February 2020.xlsx
+++ b/2020/Others/Others/Price list February 2020.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>Model</t>
   </si>
@@ -198,9 +198,6 @@
     <t xml:space="preserve">    mugdhocorporation@gmail.com</t>
   </si>
   <si>
-    <t>Address: Rozy Market, Station Bazar, Natore</t>
-  </si>
-  <si>
     <t>Discount</t>
   </si>
   <si>
@@ -282,13 +279,19 @@
     <t>D72</t>
   </si>
   <si>
-    <t>March</t>
-  </si>
-  <si>
     <t>i30</t>
   </si>
   <si>
     <t>Z50</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Address: Komola Super Market, Alaipur, Natore.</t>
+  </si>
+  <si>
+    <t>D92</t>
   </si>
 </sst>
 </file>
@@ -510,30 +513,9 @@
     <xf numFmtId="3" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,16 +542,31 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -578,14 +575,20 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -626,7 +629,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -647,7 +650,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -657,7 +660,7 @@
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="389" y="277"/>
+            <a:off x="371" y="277"/>
             <a:ext cx="16" cy="264"/>
           </a:xfrm>
           <a:custGeom>
@@ -853,7 +856,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1954,7 +1957,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2394,7 +2397,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2454,7 +2457,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2471,7 +2474,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2534,7 +2537,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2551,7 +2554,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2611,7 +2614,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2644,7 +2647,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2656,7 +2659,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2934,7 +2937,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2947,721 +2950,721 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="31" customWidth="1"/>
-    <col min="2" max="2" width="12" style="31" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="31" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="2.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12" style="6" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="11.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12" style="16" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" s="7" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A3" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30">
+        <v>2020</v>
+      </c>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="11">
+        <v>780</v>
+      </c>
+      <c r="C5" s="11">
+        <v>840</v>
+      </c>
+      <c r="D5" s="11">
+        <v>10</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1160</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1250</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11">
+        <v>800</v>
+      </c>
+      <c r="C6" s="11">
+        <v>870</v>
+      </c>
+      <c r="D6" s="11">
+        <v>10</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1010</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1090</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="11">
+        <v>790</v>
+      </c>
+      <c r="C7" s="11">
+        <v>860</v>
+      </c>
+      <c r="D7" s="11">
+        <v>10</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1040</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1130</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A8" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" s="14" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12">
-        <v>2020</v>
-      </c>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="15" t="s">
+      <c r="B8" s="11">
+        <v>740</v>
+      </c>
+      <c r="C8" s="11">
+        <v>790</v>
+      </c>
+      <c r="D8" s="11">
+        <v>10</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="13">
+        <v>970</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1050</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="11">
+        <v>800</v>
+      </c>
+      <c r="C9" s="11">
+        <v>860</v>
+      </c>
+      <c r="D9" s="11">
+        <v>10</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1100</v>
+      </c>
+      <c r="H9" s="13">
+        <v>1199</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="11">
+        <v>790</v>
+      </c>
+      <c r="C10" s="11">
+        <v>850</v>
+      </c>
+      <c r="D10" s="11">
+        <v>10</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1050</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1130</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="11">
+        <v>800</v>
+      </c>
+      <c r="C11" s="11">
+        <v>860</v>
+      </c>
+      <c r="D11" s="11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1330</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1450</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="11">
+        <v>915</v>
+      </c>
+      <c r="C12" s="11">
+        <v>990</v>
+      </c>
+      <c r="D12" s="11">
         <v>0</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="15" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="13">
+        <v>1200</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1299</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="11">
+        <v>920</v>
+      </c>
+      <c r="C13" s="11">
+        <v>999</v>
+      </c>
+      <c r="D13" s="11">
         <v>0</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="18">
-        <v>780</v>
-      </c>
-      <c r="C5" s="18">
-        <v>840</v>
-      </c>
-      <c r="D5" s="18">
+      <c r="E13" s="12"/>
+      <c r="F13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="13">
+        <v>12090</v>
+      </c>
+      <c r="H13" s="13">
+        <v>12990</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="11">
+        <v>880</v>
+      </c>
+      <c r="C14" s="11">
+        <v>950</v>
+      </c>
+      <c r="D14" s="11">
+        <v>20</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="13">
+        <v>5750</v>
+      </c>
+      <c r="H14" s="13">
+        <v>6190</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="11">
+        <v>845</v>
+      </c>
+      <c r="C15" s="11">
+        <v>910</v>
+      </c>
+      <c r="D15" s="11">
         <v>10</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="20">
-        <v>1010</v>
-      </c>
-      <c r="H5" s="20">
+      <c r="E15" s="12"/>
+      <c r="F15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1190</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1290</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A16" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="11">
+        <v>820</v>
+      </c>
+      <c r="C16" s="11">
+        <v>890</v>
+      </c>
+      <c r="D16" s="11">
+        <v>10</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="13">
+        <v>1100</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1190</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="11">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="11">
         <v>1090</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18">
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="13">
+        <v>1250</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1350</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="11">
+        <v>995</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1075</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="13">
+        <v>1370</v>
+      </c>
+      <c r="H18" s="13">
+        <v>1490</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="18">
-        <v>800</v>
-      </c>
-      <c r="C6" s="18">
-        <v>870</v>
-      </c>
-      <c r="D6" s="18">
+    <row r="19" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="13">
+        <v>880</v>
+      </c>
+      <c r="C19" s="13">
+        <v>950</v>
+      </c>
+      <c r="D19" s="11">
         <v>10</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="20">
+      <c r="E19" s="12"/>
+      <c r="F19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="13">
+        <v>3610</v>
+      </c>
+      <c r="H19" s="13">
+        <v>3890</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="11">
+        <v>900</v>
+      </c>
+      <c r="C20" s="11">
+        <v>970</v>
+      </c>
+      <c r="D20" s="11">
+        <v>10</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="4">
+        <v>3890</v>
+      </c>
+      <c r="H20" s="4">
+        <v>4190</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A21" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="13">
         <v>1040</v>
       </c>
-      <c r="H6" s="20">
-        <v>1130</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18">
+      <c r="C21" s="13">
+        <v>1120</v>
+      </c>
+      <c r="D21" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A7" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="18">
-        <v>790</v>
-      </c>
-      <c r="C7" s="18">
-        <v>860</v>
-      </c>
-      <c r="D7" s="18">
+      <c r="E21" s="12"/>
+      <c r="F21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="13">
+        <v>4280</v>
+      </c>
+      <c r="H21" s="13">
+        <v>4590</v>
+      </c>
+      <c r="I21" s="11">
+        <v>300</v>
+      </c>
+      <c r="J21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A22" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="13">
+        <v>930</v>
+      </c>
+      <c r="C22" s="13">
+        <v>999</v>
+      </c>
+      <c r="D22" s="11">
         <v>10</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="20">
-        <v>970</v>
-      </c>
-      <c r="H7" s="20">
-        <v>1050</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18">
+      <c r="E22" s="12"/>
+      <c r="F22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="13">
+        <v>5650</v>
+      </c>
+      <c r="H22" s="13">
+        <v>6150</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1190</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1290</v>
+      </c>
+      <c r="D23" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A8" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="18">
-        <v>740</v>
-      </c>
-      <c r="C8" s="18">
-        <v>790</v>
-      </c>
-      <c r="D8" s="18">
+      <c r="E23" s="12"/>
+      <c r="F23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="13">
+        <v>5020</v>
+      </c>
+      <c r="H23" s="13">
+        <v>5390</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A24" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="13">
+        <v>1170</v>
+      </c>
+      <c r="C24" s="13">
+        <v>1270</v>
+      </c>
+      <c r="D24" s="11">
         <v>10</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="20">
-        <v>1100</v>
-      </c>
-      <c r="H8" s="20">
-        <v>1199</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18">
+      <c r="E24" s="12"/>
+      <c r="F24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="13">
+        <v>5280</v>
+      </c>
+      <c r="H24" s="13">
+        <v>5690</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A25" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="13">
+        <v>4180</v>
+      </c>
+      <c r="H25" s="13">
+        <v>4490</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A26" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="13">
+        <v>1020</v>
+      </c>
+      <c r="C26" s="13">
+        <v>1090</v>
+      </c>
+      <c r="D26" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="18">
-        <v>800</v>
-      </c>
-      <c r="C9" s="18">
-        <v>860</v>
-      </c>
-      <c r="D9" s="18">
-        <v>10</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="20">
-        <v>1050</v>
-      </c>
-      <c r="H9" s="20">
-        <v>1130</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A10" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="18">
-        <v>790</v>
-      </c>
-      <c r="C10" s="18">
-        <v>850</v>
-      </c>
-      <c r="D10" s="18">
-        <v>10</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="20">
-        <v>1330</v>
-      </c>
-      <c r="H10" s="20">
-        <v>1450</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A11" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="18">
-        <v>800</v>
-      </c>
-      <c r="C11" s="18">
-        <v>860</v>
-      </c>
-      <c r="D11" s="18">
-        <v>10</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="20">
-        <v>1200</v>
-      </c>
-      <c r="H11" s="20">
-        <v>1299</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A12" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="18">
-        <v>915</v>
-      </c>
-      <c r="C12" s="18">
-        <v>990</v>
-      </c>
-      <c r="D12" s="18">
+      <c r="E26" s="12"/>
+      <c r="F26" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="13">
+        <v>5100</v>
+      </c>
+      <c r="H26" s="13">
+        <v>5490</v>
+      </c>
+      <c r="I26" s="11">
+        <v>70</v>
+      </c>
+      <c r="J26" s="11">
         <v>0</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="20">
-        <v>12090</v>
-      </c>
-      <c r="H12" s="20">
-        <v>12990</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A13" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="18">
-        <v>920</v>
-      </c>
-      <c r="C13" s="18">
-        <v>999</v>
-      </c>
-      <c r="D13" s="18">
-        <v>0</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="20">
-        <v>5750</v>
-      </c>
-      <c r="H13" s="20">
-        <v>6190</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A14" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="18">
-        <v>880</v>
-      </c>
-      <c r="C14" s="18">
-        <v>950</v>
-      </c>
-      <c r="D14" s="18">
-        <v>20</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="20">
-        <v>1190</v>
-      </c>
-      <c r="H14" s="20">
-        <v>1290</v>
-      </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="18">
-        <v>845</v>
-      </c>
-      <c r="C15" s="18">
-        <v>910</v>
-      </c>
-      <c r="D15" s="18">
-        <v>10</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="20">
-        <v>1100</v>
-      </c>
-      <c r="H15" s="20">
-        <v>1190</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A16" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="18">
-        <v>820</v>
-      </c>
-      <c r="C16" s="18">
-        <v>890</v>
-      </c>
-      <c r="D16" s="18">
-        <v>10</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="20">
-        <v>1250</v>
-      </c>
-      <c r="H16" s="20">
-        <v>1350</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="18">
-        <v>1000</v>
-      </c>
-      <c r="C17" s="18">
-        <v>1090</v>
-      </c>
-      <c r="D17" s="18">
-        <v>0</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="20">
-        <v>1370</v>
-      </c>
-      <c r="H17" s="20">
-        <v>1490</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A18" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="18">
-        <v>995</v>
-      </c>
-      <c r="C18" s="18">
-        <v>1075</v>
-      </c>
-      <c r="D18" s="18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="G18" s="20">
-        <v>3610</v>
-      </c>
-      <c r="H18" s="20">
-        <v>3890</v>
-      </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A19" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="20">
-        <v>880</v>
-      </c>
-      <c r="C19" s="20">
-        <v>950</v>
-      </c>
-      <c r="D19" s="18">
-        <v>10</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="20">
-        <v>3890</v>
-      </c>
-      <c r="H19" s="20">
-        <v>4190</v>
-      </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A20" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="18">
-        <v>900</v>
-      </c>
-      <c r="C20" s="18">
-        <v>970</v>
-      </c>
-      <c r="D20" s="18">
-        <v>10</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="4">
-        <v>4280</v>
-      </c>
-      <c r="H20" s="4">
-        <v>4590</v>
-      </c>
-      <c r="I20" s="3">
-        <v>300</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="20">
-        <v>1040</v>
-      </c>
-      <c r="C21" s="20">
-        <v>1120</v>
-      </c>
-      <c r="D21" s="18">
-        <v>20</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="20">
-        <v>5650</v>
-      </c>
-      <c r="H21" s="20">
-        <v>6150</v>
-      </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A22" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="20">
-        <v>930</v>
-      </c>
-      <c r="C22" s="20">
-        <v>999</v>
-      </c>
-      <c r="D22" s="18">
-        <v>10</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="20">
-        <v>5020</v>
-      </c>
-      <c r="H22" s="20">
-        <v>5390</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A23" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="20">
-        <v>1190</v>
-      </c>
-      <c r="C23" s="20">
-        <v>1290</v>
-      </c>
-      <c r="D23" s="18">
-        <v>10</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="20">
-        <v>5280</v>
-      </c>
-      <c r="H23" s="20">
-        <v>5690</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A24" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="20">
-        <v>1170</v>
-      </c>
-      <c r="C24" s="20">
-        <v>1270</v>
-      </c>
-      <c r="D24" s="18">
-        <v>10</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="20">
-        <v>4180</v>
-      </c>
-      <c r="H24" s="20">
-        <v>4490</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A25" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="20">
-        <v>5100</v>
-      </c>
-      <c r="H25" s="20">
-        <v>5490</v>
-      </c>
-      <c r="I25" s="18">
-        <v>70</v>
-      </c>
-      <c r="J25" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A26" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="20">
-        <v>2780</v>
-      </c>
-      <c r="C26" s="20">
-        <v>2990</v>
-      </c>
-      <c r="D26" s="18">
-        <v>450</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="20">
-        <v>5390</v>
-      </c>
-      <c r="H26" s="20">
-        <v>5790</v>
-      </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18">
-        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="19.5" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B27" s="4">
-        <v>2770</v>
+        <v>2780</v>
       </c>
       <c r="C27" s="4">
         <v>2990</v>
@@ -3669,442 +3672,456 @@
       <c r="D27" s="3">
         <v>450</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="18" t="s">
+      <c r="E27" s="12"/>
+      <c r="F27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="13">
+        <v>5390</v>
+      </c>
+      <c r="H27" s="13">
+        <v>5790</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="13">
+        <v>2770</v>
+      </c>
+      <c r="C28" s="13">
+        <v>2990</v>
+      </c>
+      <c r="D28" s="11">
+        <v>450</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G28" s="4">
         <v>3560</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H28" s="4">
         <v>3840</v>
       </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18">
+      <c r="I28" s="3"/>
+      <c r="J28" s="11">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A28" s="18" t="s">
+    <row r="29" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A29" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="13">
+        <v>6540</v>
+      </c>
+      <c r="C29" s="13">
+        <v>6990</v>
+      </c>
+      <c r="D29" s="11">
+        <v>70</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="13">
+        <v>3340</v>
+      </c>
+      <c r="H29" s="13">
+        <v>3590</v>
+      </c>
+      <c r="I29" s="11">
+        <v>600</v>
+      </c>
+      <c r="J29" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A30" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="13">
+        <v>8340</v>
+      </c>
+      <c r="C30" s="13">
+        <v>8990</v>
+      </c>
+      <c r="D30" s="11">
+        <v>2000</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="13">
+        <v>4500</v>
+      </c>
+      <c r="H30" s="13">
+        <v>4790</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="13">
+        <v>9190</v>
+      </c>
+      <c r="C31" s="13">
+        <v>9990</v>
+      </c>
+      <c r="D31" s="11">
+        <v>170</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="13">
+        <v>4970</v>
+      </c>
+      <c r="H31" s="13">
+        <v>5290</v>
+      </c>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="19.5" customHeight="1">
+      <c r="A32" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="20">
-        <v>6540</v>
-      </c>
-      <c r="C28" s="20">
-        <v>6990</v>
-      </c>
-      <c r="D28" s="18">
-        <v>70</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="4">
-        <v>3340</v>
-      </c>
-      <c r="H28" s="4">
-        <v>3590</v>
-      </c>
-      <c r="I28" s="3">
-        <v>600</v>
-      </c>
-      <c r="J28" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A29" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="20">
-        <v>8340</v>
-      </c>
-      <c r="C29" s="20">
-        <v>8990</v>
-      </c>
-      <c r="D29" s="18">
-        <v>2000</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="20">
-        <v>4500</v>
-      </c>
-      <c r="H29" s="20">
-        <v>4790</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A30" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="20">
-        <v>9190</v>
-      </c>
-      <c r="C30" s="20">
-        <v>9990</v>
-      </c>
-      <c r="D30" s="18">
-        <v>170</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="20">
-        <v>4970</v>
-      </c>
-      <c r="H30" s="20">
+      <c r="B32" s="13">
         <v>5290</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A31" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="20">
-        <v>5290</v>
-      </c>
-      <c r="C31" s="20">
+      <c r="C32" s="13">
         <v>5690</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D32" s="11">
         <v>80</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="18" t="s">
+      <c r="E32" s="12"/>
+      <c r="F32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G32" s="4">
         <v>3710</v>
       </c>
-      <c r="H31" s="20">
+      <c r="H32" s="4">
         <v>3990</v>
       </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18">
+      <c r="I32" s="3"/>
+      <c r="J32" s="11">
         <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A32" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="20">
-        <v>5010</v>
-      </c>
-      <c r="C32" s="20">
-        <v>5390</v>
-      </c>
-      <c r="D32" s="18">
-        <v>70</v>
-      </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="4">
-        <v>3620</v>
-      </c>
-      <c r="H32" s="4">
-        <v>3890</v>
-      </c>
-      <c r="I32" s="3">
-        <v>600</v>
-      </c>
-      <c r="J32" s="18">
-        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="19.5" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B33" s="4">
-        <v>5170</v>
+        <v>5010</v>
       </c>
       <c r="C33" s="4">
-        <v>5499</v>
+        <v>5390</v>
       </c>
       <c r="D33" s="3">
+        <v>70</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="13">
+        <v>3620</v>
+      </c>
+      <c r="H33" s="13">
+        <v>3890</v>
+      </c>
+      <c r="I33" s="11">
+        <v>600</v>
+      </c>
+      <c r="J33" s="11">
         <v>50</v>
-      </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G33" s="20">
-        <v>4080</v>
-      </c>
-      <c r="H33" s="20">
-        <v>4390</v>
-      </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18">
-        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="19.5" customHeight="1">
       <c r="A34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="4">
+        <v>5170</v>
+      </c>
+      <c r="C34" s="4">
+        <v>5499</v>
+      </c>
+      <c r="D34" s="3">
+        <v>50</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="13">
+        <v>4080</v>
+      </c>
+      <c r="H34" s="13">
+        <v>4390</v>
+      </c>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A35" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="13">
+        <v>5750</v>
+      </c>
+      <c r="C35" s="13">
+        <v>6190</v>
+      </c>
+      <c r="D35" s="11">
+        <v>550</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="13">
+        <v>4220</v>
+      </c>
+      <c r="H35" s="13">
+        <v>4540</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A36" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="4">
-        <v>5750</v>
-      </c>
-      <c r="C34" s="4">
-        <v>6190</v>
-      </c>
-      <c r="D34" s="3">
-        <v>550</v>
-      </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="20">
-        <v>4220</v>
-      </c>
-      <c r="H34" s="20">
-        <v>4540</v>
-      </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18">
+      <c r="B36" s="13">
+        <v>5550</v>
+      </c>
+      <c r="C36" s="13">
+        <v>5990</v>
+      </c>
+      <c r="D36" s="11">
+        <v>60</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="13">
+        <v>3710</v>
+      </c>
+      <c r="H36" s="13">
+        <v>3990</v>
+      </c>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A35" s="18" t="s">
+    <row r="37" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A37" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="20">
-        <v>5550</v>
-      </c>
-      <c r="C35" s="20">
+      <c r="B37" s="13">
+        <v>5940</v>
+      </c>
+      <c r="C37" s="13">
+        <v>6390</v>
+      </c>
+      <c r="D37" s="11">
+        <v>90</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="13">
+        <v>7350</v>
+      </c>
+      <c r="H37" s="13">
+        <v>7990</v>
+      </c>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A38" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="13">
+        <v>5940</v>
+      </c>
+      <c r="C38" s="13">
+        <v>6390</v>
+      </c>
+      <c r="D38" s="11">
+        <v>90</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="13">
+        <v>7890</v>
+      </c>
+      <c r="H38" s="13">
+        <v>8490</v>
+      </c>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A39" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="13">
+        <v>5510</v>
+      </c>
+      <c r="C39" s="13">
         <v>5990</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D39" s="11">
         <v>60</v>
       </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G35" s="20">
-        <v>3710</v>
-      </c>
-      <c r="H35" s="20">
-        <v>3990</v>
-      </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18">
+      <c r="E39" s="12"/>
+      <c r="F39" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="13">
+        <v>8310</v>
+      </c>
+      <c r="H39" s="13">
+        <v>8990</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A40" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="13">
+        <v>6470</v>
+      </c>
+      <c r="C40" s="13">
+        <v>6990</v>
+      </c>
+      <c r="D40" s="11">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A36" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="20">
-        <v>5940</v>
-      </c>
-      <c r="C36" s="20">
-        <v>6390</v>
-      </c>
-      <c r="D36" s="18">
-        <v>90</v>
-      </c>
-      <c r="E36" s="19"/>
-      <c r="F36" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G36" s="20">
-        <v>7350</v>
-      </c>
-      <c r="H36" s="20">
-        <v>7990</v>
-      </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18">
+      <c r="E40" s="12"/>
+      <c r="F40" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="13">
+        <v>8310</v>
+      </c>
+      <c r="H40" s="13">
+        <v>8990</v>
+      </c>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A37" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="20">
-        <v>5940</v>
-      </c>
-      <c r="C37" s="20">
-        <v>6390</v>
-      </c>
-      <c r="D37" s="18">
-        <v>90</v>
-      </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" s="20">
-        <v>7890</v>
-      </c>
-      <c r="H37" s="20">
-        <v>8490</v>
-      </c>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18">
+    <row r="41" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A41" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="13">
+        <v>1220</v>
+      </c>
+      <c r="C41" s="13">
+        <v>1320</v>
+      </c>
+      <c r="D41" s="11">
+        <v>20</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" s="13">
+        <v>10340</v>
+      </c>
+      <c r="H41" s="13">
+        <v>10990</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A38" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="20">
-        <v>6030</v>
-      </c>
-      <c r="C38" s="20">
-        <v>6490</v>
-      </c>
-      <c r="D38" s="18">
-        <v>60</v>
-      </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" s="20">
-        <v>8310</v>
-      </c>
-      <c r="H38" s="20">
-        <v>8990</v>
-      </c>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A39" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="20">
-        <v>6470</v>
-      </c>
-      <c r="C39" s="20">
-        <v>6990</v>
-      </c>
-      <c r="D39" s="18">
+    <row r="42" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A42" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G39" s="20">
-        <v>8310</v>
-      </c>
-      <c r="H39" s="20">
-        <v>8990</v>
-      </c>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A40" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="20">
-        <v>1220</v>
-      </c>
-      <c r="C40" s="20">
-        <v>1320</v>
-      </c>
-      <c r="D40" s="18">
+      <c r="B42" s="13">
+        <v>1070</v>
+      </c>
+      <c r="C42" s="13">
+        <v>1160</v>
+      </c>
+      <c r="D42" s="11">
         <v>20</v>
       </c>
-      <c r="E40" s="19"/>
-      <c r="F40" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A41" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="20">
-        <v>1070</v>
-      </c>
-      <c r="C41" s="20">
-        <v>1160</v>
-      </c>
-      <c r="D41" s="18">
+      <c r="E42" s="12"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="1:11" ht="19.5" customHeight="1">
+      <c r="A43" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="13">
+        <v>1100</v>
+      </c>
+      <c r="C43" s="13">
+        <v>1199</v>
+      </c>
+      <c r="D43" s="11">
         <v>20</v>
       </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-    </row>
-    <row r="42" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A42" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="20">
-        <v>1100</v>
-      </c>
-      <c r="C42" s="20">
-        <v>1199</v>
-      </c>
-      <c r="D42" s="18">
-        <v>20</v>
-      </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-    </row>
-    <row r="43" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A43" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="20">
-        <v>1160</v>
-      </c>
-      <c r="C43" s="20">
-        <v>1250</v>
-      </c>
-      <c r="D43" s="18">
-        <v>20</v>
-      </c>
-      <c r="E43" s="19"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
     </row>
     <row r="44" spans="1:11" ht="15.75">
       <c r="A44" s="23" t="s">
@@ -4112,30 +4129,30 @@
       </c>
       <c r="B44" s="24"/>
       <c r="C44" s="24" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
-      <c r="H44" s="25" t="s">
+      <c r="H44" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="I44" s="25"/>
-      <c r="J44" s="26"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="20"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="30"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11">

</xml_diff>